<commit_message>
TS Jatai working 13/06/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Rule Processing Table.xlsx
+++ b/TS Jatai Working/Rule Processing Table.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="634">
   <si>
     <t>Special Rules Tables for Rajadhiraaja</t>
   </si>
@@ -759,9 +759,6 @@
     <t>nEShTaH</t>
   </si>
   <si>
-    <t xml:space="preserve"> tvaShTaH</t>
-  </si>
-  <si>
     <t>kaH</t>
   </si>
   <si>
@@ -777,9 +774,6 @@
     <t>antaH</t>
   </si>
   <si>
-    <t>No swaram on first letter</t>
-  </si>
-  <si>
     <t>ahAH</t>
   </si>
   <si>
@@ -1921,6 +1915,18 @@
   </si>
   <si>
     <t>H =Sh</t>
+  </si>
+  <si>
+    <t>tvaShTaH</t>
+  </si>
+  <si>
+    <t>a = anudAttam</t>
+  </si>
+  <si>
+    <t>else o</t>
+  </si>
+  <si>
+    <t>udAttam = o</t>
   </si>
 </sst>
 </file>
@@ -2352,10 +2358,10 @@
   <dimension ref="A3:T237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E184" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E169" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F229" sqref="F229"/>
+      <selection pane="bottomRight" activeCell="E212" sqref="E212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2413,34 +2419,34 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>281</v>
-      </c>
       <c r="K5" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2469,16 +2475,16 @@
         <v>129</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2507,16 +2513,16 @@
         <v>130</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2545,7 +2551,7 @@
         <v>131</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>6</v>
@@ -2554,7 +2560,7 @@
         <v>13</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2583,7 +2589,7 @@
         <v>133</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>15</v>
@@ -2592,7 +2598,7 @@
         <v>16</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2621,7 +2627,7 @@
         <v>132</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>18</v>
@@ -2630,7 +2636,7 @@
         <v>19</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2680,7 +2686,7 @@
         <v>128</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>15</v>
@@ -2689,7 +2695,7 @@
         <v>201</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2703,34 +2709,34 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="L13" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2759,19 +2765,19 @@
         <v>26</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
@@ -2800,19 +2806,19 @@
         <v>26</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M15" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.4">
@@ -2829,10 +2835,10 @@
         <v>30</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>31</v>
@@ -2844,19 +2850,19 @@
         <v>8</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2884,32 +2890,32 @@
         <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="T18" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2929,17 +2935,17 @@
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>34</v>
@@ -2948,22 +2954,22 @@
         <v>35</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2980,7 +2986,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>35</v>
@@ -3023,7 +3029,7 @@
         <v>164</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>37</v>
@@ -3033,22 +3039,22 @@
         <v>37</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3075,7 +3081,7 @@
       </c>
       <c r="I22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>34</v>
@@ -3090,16 +3096,16 @@
         <v>36</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3122,35 +3128,35 @@
         <v>40</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I23" s="2"/>
       <c r="K23" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M23" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="Q23" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="S23" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3244,7 +3250,7 @@
         <v>148</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>12</v>
@@ -3260,25 +3266,25 @@
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P30" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q30" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3292,7 +3298,7 @@
         <v>148</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>12</v>
@@ -3308,25 +3314,25 @@
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M31" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q31" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3350,7 +3356,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>149</v>
@@ -3372,16 +3378,16 @@
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M33" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3414,16 +3420,16 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>150</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3456,16 +3462,16 @@
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L35" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="O35" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3498,16 +3504,16 @@
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="O36" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3540,16 +3546,16 @@
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L37" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="M37" s="2" t="s">
-        <v>401</v>
-      </c>
       <c r="O37" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3582,16 +3588,16 @@
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>154</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3624,16 +3630,16 @@
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>155</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3666,7 +3672,7 @@
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>156</v>
@@ -3675,7 +3681,7 @@
         <v>153</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3686,7 +3692,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>157</v>
@@ -3708,16 +3714,16 @@
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L41" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="O41" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3750,16 +3756,16 @@
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>158</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3822,16 +3828,16 @@
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>160</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3845,7 +3851,7 @@
         <v>24</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>12</v>
@@ -3864,16 +3870,16 @@
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3884,10 +3890,10 @@
         <v>32</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>12</v>
@@ -3906,16 +3912,16 @@
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L46" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3926,7 +3932,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>161</v>
@@ -3948,16 +3954,16 @@
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L47" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3990,16 +3996,16 @@
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>162</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4013,7 +4019,7 @@
         <v>24</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>12</v>
@@ -4032,16 +4038,16 @@
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4074,16 +4080,16 @@
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>152</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4094,7 +4100,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>153</v>
@@ -4116,16 +4122,16 @@
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4158,16 +4164,16 @@
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>158</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4198,7 +4204,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>12</v>
@@ -4210,21 +4216,21 @@
         <v>142</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="O55" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4238,7 +4244,7 @@
         <v>2</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>12</v>
@@ -4250,21 +4256,21 @@
         <v>142</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4278,7 +4284,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>12</v>
@@ -4290,21 +4296,21 @@
         <v>142</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="O57" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4335,16 +4341,16 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>136</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4375,16 +4381,16 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L59" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="O59" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4415,16 +4421,16 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>138</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4438,7 +4444,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>12</v>
@@ -4450,28 +4456,28 @@
         <v>142</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K61" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="M61" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="L61" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>438</v>
-      </c>
       <c r="N61" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>139</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4501,25 +4507,25 @@
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="N63" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4545,25 +4551,25 @@
         <v>70</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="L64" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="N64" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>61</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="Q64" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4589,25 +4595,25 @@
         <v>70</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N65" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="P65" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="O65" s="2" t="s">
+      <c r="Q65" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="P65" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="Q65" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4633,25 +4639,25 @@
         <v>70</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N66" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="O66" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="P66" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="O66" s="2" t="s">
+      <c r="Q66" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="P66" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q66" s="2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4677,7 +4683,7 @@
         <v>70</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>26</v>
@@ -4686,7 +4692,7 @@
         <v>6</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4712,7 +4718,7 @@
         <v>70</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>64</v>
@@ -4721,7 +4727,7 @@
         <v>6</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4747,7 +4753,7 @@
         <v>70</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>65</v>
@@ -4756,7 +4762,7 @@
         <v>6</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4782,7 +4788,7 @@
         <v>70</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4808,16 +4814,16 @@
         <v>70</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>67</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4843,16 +4849,16 @@
         <v>70</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>68</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4878,16 +4884,16 @@
         <v>70</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>69</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4913,22 +4919,22 @@
         <v>146</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L74" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M74" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="N74" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="P74" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4954,22 +4960,22 @@
         <v>146</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>147</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4995,17 +5001,17 @@
         <v>70</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>71</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5031,17 +5037,17 @@
         <v>70</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>72</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5052,7 +5058,7 @@
         <v>24</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>12</v>
@@ -5067,17 +5073,17 @@
         <v>70</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="L78" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="M78" s="2" t="s">
         <v>517</v>
-      </c>
-      <c r="M78" s="2" t="s">
-        <v>519</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5103,17 +5109,17 @@
         <v>70</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5139,17 +5145,17 @@
         <v>70</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>74</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5175,17 +5181,17 @@
         <v>70</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>75</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5196,7 +5202,7 @@
         <v>24</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>12</v>
@@ -5211,25 +5217,25 @@
         <v>70</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M82" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="O82" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="P82" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="N82" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="O82" s="2" t="s">
+      <c r="Q82" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="P82" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="Q82" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5255,17 +5261,17 @@
         <v>70</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>76</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5291,17 +5297,17 @@
         <v>70</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>77</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5327,16 +5333,16 @@
         <v>70</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>78</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5362,16 +5368,16 @@
         <v>70</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5397,16 +5403,16 @@
         <v>70</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>80</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5433,13 +5439,13 @@
         <v>86</v>
       </c>
       <c r="J88" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="L88" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5465,19 +5471,19 @@
         <v>86</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>77</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5488,7 +5494,7 @@
         <v>24</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>29</v>
@@ -5503,13 +5509,13 @@
         <v>86</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5720,7 +5726,7 @@
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>142</v>
@@ -5755,35 +5761,35 @@
         <v>24</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>142</v>
       </c>
       <c r="H105" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="J105" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="K105" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="J105" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="K105" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="L105" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="M105" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="O105" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="M105" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="O105" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5798,7 +5804,7 @@
         <v>164</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>142</v>
@@ -5817,7 +5823,7 @@
         <v>164</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>142</v>
@@ -5832,26 +5838,26 @@
         <v>135</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G108" s="2"/>
       <c r="I108" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5862,26 +5868,26 @@
         <v>135</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G109" s="2"/>
       <c r="I109" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6419,7 +6425,7 @@
         <v>32</v>
       </c>
       <c r="C134" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>114</v>
@@ -6445,7 +6451,7 @@
         <v>32</v>
       </c>
       <c r="C135" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>114</v>
@@ -6471,7 +6477,7 @@
         <v>32</v>
       </c>
       <c r="C136" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>114</v>
@@ -6497,7 +6503,7 @@
         <v>32</v>
       </c>
       <c r="C137" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>114</v>
@@ -6523,7 +6529,7 @@
         <v>32</v>
       </c>
       <c r="C138" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>114</v>
@@ -6549,7 +6555,7 @@
         <v>32</v>
       </c>
       <c r="C139" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>114</v>
@@ -6858,31 +6864,31 @@
         <v>43</v>
       </c>
       <c r="I157" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="J157" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="K157" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="J157" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="K157" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="L157" s="2" t="s">
         <v>206</v>
       </c>
       <c r="M157" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="N157" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="O157" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="P157" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="N157" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="O157" s="2" t="s">
+      <c r="Q157" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="P157" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="Q157" s="2" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="158" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6914,19 +6920,19 @@
         <v>193</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K158" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L158" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="M158" s="2" t="s">
         <v>193</v>
       </c>
       <c r="O158" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="159" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6955,22 +6961,22 @@
         <v>43</v>
       </c>
       <c r="I159" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="J159" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="K159" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="L159" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="O159" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="J159" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="K159" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="L159" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="M159" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="O159" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="160" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7002,19 +7008,19 @@
         <v>195</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K160" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L160" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M160" s="2" t="s">
         <v>195</v>
       </c>
       <c r="O160" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="161" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7046,28 +7052,28 @@
         <v>196</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K161" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="L161" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="M161" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="N161" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="L161" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="M161" s="2" t="s">
+      <c r="O161" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="N161" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="O161" s="2" t="s">
-        <v>583</v>
       </c>
       <c r="P161" s="2" t="s">
         <v>196</v>
       </c>
       <c r="Q161" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="162" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7099,19 +7105,19 @@
         <v>197</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L162" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M162" s="2" t="s">
         <v>197</v>
       </c>
       <c r="O162" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7140,7 +7146,7 @@
         <v>43</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="164" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7172,19 +7178,19 @@
         <v>199</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L164" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M164" s="2" t="s">
         <v>199</v>
       </c>
       <c r="O164" s="2" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="165" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7216,19 +7222,19 @@
         <v>200</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L165" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M165" s="2" t="s">
         <v>200</v>
       </c>
       <c r="O165" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="166" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7245,10 +7251,10 @@
         <v>43</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>209</v>
@@ -7257,27 +7263,27 @@
         <v>43</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="K166" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L166" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M166" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="O166" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="167" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>32</v>
@@ -7289,34 +7295,34 @@
         <v>55</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H167" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I167" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="J167" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="K167" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="J167" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="K167" s="2" t="s">
-        <v>615</v>
       </c>
       <c r="L167" s="2" t="s">
         <v>158</v>
       </c>
       <c r="M167" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="O167" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="168" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7348,19 +7354,19 @@
         <v>201</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L168" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="M168" s="2" t="s">
         <v>201</v>
       </c>
       <c r="O168" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="169" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7392,19 +7398,19 @@
         <v>202</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="K169" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L169" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="M169" s="2" t="s">
         <v>202</v>
       </c>
       <c r="O169" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="170" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7436,19 +7442,19 @@
         <v>203</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="M170" s="2" t="s">
         <v>203</v>
       </c>
       <c r="O170" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="171" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7480,10 +7486,10 @@
         <v>204</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="K171" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L171" s="2" t="s">
         <v>153</v>
@@ -7492,7 +7498,7 @@
         <v>204</v>
       </c>
       <c r="O171" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="172" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7524,19 +7530,19 @@
         <v>205</v>
       </c>
       <c r="J172" s="11" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L172" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="M172" s="11" t="s">
         <v>205</v>
       </c>
       <c r="O172" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="173" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7568,19 +7574,19 @@
         <v>207</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K173" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L173" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="M173" s="2" t="s">
         <v>207</v>
       </c>
       <c r="O173" s="2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="174" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8202,7 +8208,7 @@
         <v>24</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>244</v>
+        <v>630</v>
       </c>
       <c r="G210" s="2" t="s">
         <v>219</v>
@@ -8219,13 +8225,13 @@
         <v>24</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E211" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G211" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="G211" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8239,13 +8245,13 @@
         <v>24</v>
       </c>
       <c r="D212" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E212" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E212" s="2" t="s">
+      <c r="G212" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="G212" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -8259,13 +8265,16 @@
         <v>24</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>250</v>
+        <v>631</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>632</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8276,13 +8285,13 @@
         <v>32</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G214" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8293,13 +8302,13 @@
         <v>32</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>225</v>
       </c>
       <c r="G215" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8310,13 +8319,13 @@
         <v>32</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>228</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8327,16 +8336,16 @@
         <v>32</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F217" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8347,16 +8356,16 @@
         <v>32</v>
       </c>
       <c r="C218" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F218" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D218" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F218" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="G218" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8367,16 +8376,16 @@
         <v>32</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F219" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G219" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8387,16 +8396,16 @@
         <v>32</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F220" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G220" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8407,16 +8416,16 @@
         <v>32</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="222" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8427,16 +8436,16 @@
         <v>32</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F222" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G222" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="223" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8447,16 +8456,16 @@
         <v>32</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F223" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G223" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8467,16 +8476,16 @@
         <v>32</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F224" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="225" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8487,16 +8496,16 @@
         <v>32</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F225" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="226" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8507,16 +8516,16 @@
         <v>32</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F226" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8527,16 +8536,16 @@
         <v>32</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F227" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8550,16 +8559,16 @@
         <v>24</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8573,16 +8582,16 @@
         <v>24</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F229" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8596,16 +8605,16 @@
         <v>59</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F230" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8619,10 +8628,10 @@
         <v>148</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="232" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8636,10 +8645,10 @@
         <v>2</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8653,10 +8662,10 @@
         <v>2</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8670,16 +8679,16 @@
         <v>148</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E234" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F234" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G234" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8693,16 +8702,16 @@
         <v>2</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E235" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F235" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G235" s="2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="236" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8725,7 +8734,7 @@
         <v>229</v>
       </c>
       <c r="G236" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8745,10 +8754,10 @@
         <v>12</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G237" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TS Jatai working 08/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Rule Processing Table.xlsx
+++ b/TS Jatai Working/Rule Processing Table.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="1108">
   <si>
     <t>Special Rules Tables for Rajadhiraaja</t>
   </si>
@@ -3363,6 +3363,12 @@
   </si>
   <si>
     <t xml:space="preserve">doShAvastaH </t>
+  </si>
+  <si>
+    <t>iH</t>
+  </si>
+  <si>
+    <t>H=Sh</t>
   </si>
 </sst>
 </file>
@@ -3500,7 +3506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3547,6 +3553,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3827,13 +3834,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V286"/>
+  <dimension ref="A3:V287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D240" sqref="D240"/>
+      <selection pane="bottomRight" activeCell="D272" sqref="D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13121,34 +13128,26 @@
       <c r="B272" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C272" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D272" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E272" s="2" t="s">
+      <c r="C272" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="D272" s="32" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E272" s="32" t="s">
         <v>1006</v>
       </c>
-      <c r="F272" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G272" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="K272" s="2" t="s">
-        <v>993</v>
-      </c>
-      <c r="L272" s="2" t="s">
-        <v>994</v>
-      </c>
-      <c r="M272" s="2" t="s">
-        <v>219</v>
-      </c>
+      <c r="F272" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="G272" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="K272" s="2"/>
+      <c r="L272" s="2"/>
+      <c r="M272" s="2"/>
       <c r="N272" s="2"/>
-      <c r="O272" s="2" t="s">
-        <v>995</v>
-      </c>
+      <c r="O272" s="2"/>
     </row>
     <row r="273" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
@@ -13167,23 +13166,23 @@
         <v>1006</v>
       </c>
       <c r="F273" s="2" t="s">
-        <v>1005</v>
+        <v>219</v>
       </c>
       <c r="G273" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K273" s="2" t="s">
-        <v>1004</v>
+        <v>993</v>
       </c>
       <c r="L273" s="2" t="s">
-        <v>227</v>
+        <v>994</v>
       </c>
       <c r="M273" s="2" t="s">
-        <v>1005</v>
+        <v>219</v>
       </c>
       <c r="N273" s="2"/>
       <c r="O273" s="2" t="s">
-        <v>1008</v>
+        <v>995</v>
       </c>
     </row>
     <row r="274" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13197,29 +13196,29 @@
         <v>214</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E274" s="2" t="s">
         <v>1006</v>
       </c>
       <c r="F274" s="2" t="s">
-        <v>84</v>
+        <v>1005</v>
       </c>
       <c r="G274" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K274" s="2" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="L274" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="M274" s="2" t="s">
-        <v>84</v>
+        <v>1005</v>
       </c>
       <c r="N274" s="2"/>
       <c r="O274" s="2" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="275" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13233,29 +13232,29 @@
         <v>214</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>107</v>
+        <v>1006</v>
       </c>
       <c r="F275" s="2" t="s">
-        <v>225</v>
+        <v>84</v>
       </c>
       <c r="G275" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K275" s="2" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="L275" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M275" s="2" t="s">
-        <v>1011</v>
+        <v>84</v>
       </c>
       <c r="N275" s="2"/>
       <c r="O275" s="2" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="276" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13266,32 +13265,32 @@
         <v>31</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>23</v>
+        <v>214</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E276" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G276" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K276" s="2" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="L276" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M276" s="2" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="N276" s="2"/>
       <c r="O276" s="2" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="277" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13305,28 +13304,29 @@
         <v>23</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E277" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G277" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K277" s="2" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="L277" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M277" s="2" t="s">
-        <v>1017</v>
-      </c>
+        <v>1014</v>
+      </c>
+      <c r="N277" s="2"/>
       <c r="O277" s="2" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="278" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13337,31 +13337,31 @@
         <v>31</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E278" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F278" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G278" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K278" s="2" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="L278" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M278" s="2" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="O278" s="2" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="279" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13372,30 +13372,31 @@
         <v>31</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>963</v>
+        <v>51</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E279" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="F279" s="2" t="s">
-        <v>958</v>
+        <v>231</v>
       </c>
       <c r="G279" s="2" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="K279" s="2" t="s">
-        <v>959</v>
+        <v>1019</v>
       </c>
       <c r="L279" s="2" t="s">
-        <v>960</v>
+        <v>228</v>
       </c>
       <c r="M279" s="2" t="s">
-        <v>958</v>
-      </c>
-      <c r="N279" s="2"/>
+        <v>1020</v>
+      </c>
       <c r="O279" s="2" t="s">
-        <v>961</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="280" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13403,40 +13404,33 @@
         <v>187</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>658</v>
+        <v>963</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>1023</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E280" s="2"/>
       <c r="F280" s="2" t="s">
-        <v>84</v>
+        <v>958</v>
       </c>
       <c r="G280" s="2" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="K280" s="2" t="s">
-        <v>1022</v>
+        <v>959</v>
       </c>
       <c r="L280" s="2" t="s">
-        <v>1024</v>
+        <v>960</v>
       </c>
       <c r="M280" s="2" t="s">
-        <v>1025</v>
-      </c>
-      <c r="N280" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>958</v>
+      </c>
+      <c r="N280" s="2"/>
       <c r="O280" s="2" t="s">
-        <v>1026</v>
-      </c>
-      <c r="P280" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="Q280" s="2" t="s">
-        <v>1028</v>
+        <v>961</v>
       </c>
     </row>
     <row r="281" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13447,30 +13441,37 @@
         <v>115</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D281" s="2"/>
-      <c r="E281" s="2" t="s">
-        <v>23</v>
+        <v>658</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>1023</v>
       </c>
       <c r="F281" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G281" s="2" t="s">
         <v>220</v>
       </c>
       <c r="K281" s="2" t="s">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="L281" s="2" t="s">
-        <v>212</v>
+        <v>1024</v>
       </c>
       <c r="M281" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N281" s="2"/>
+        <v>1025</v>
+      </c>
+      <c r="N281" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="O281" s="2" t="s">
-        <v>1030</v>
+        <v>1026</v>
+      </c>
+      <c r="P281" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Q281" s="2" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="282" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13483,29 +13484,28 @@
       <c r="C282" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D282" s="2" t="s">
-        <v>232</v>
-      </c>
+      <c r="D282" s="2"/>
       <c r="E282" s="2" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>979</v>
+        <v>86</v>
       </c>
       <c r="G282" s="2" t="s">
         <v>220</v>
       </c>
       <c r="K282" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="L282" s="2" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="M282" s="2" t="s">
-        <v>979</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="N282" s="2"/>
       <c r="O282" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="283" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13516,40 +13516,31 @@
         <v>115</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>658</v>
+        <v>2</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>957</v>
+        <v>232</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="F283" s="2" t="s">
-        <v>233</v>
+        <v>979</v>
       </c>
       <c r="G283" s="2" t="s">
         <v>220</v>
       </c>
       <c r="K283" s="2" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="L283" s="2" t="s">
-        <v>1035</v>
+        <v>232</v>
       </c>
       <c r="M283" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="N283" s="2" t="s">
-        <v>233</v>
+        <v>979</v>
       </c>
       <c r="O283" s="2" t="s">
-        <v>1036</v>
-      </c>
-      <c r="P283" s="8" t="s">
-        <v>1037</v>
-      </c>
-      <c r="Q283" s="2" t="s">
-        <v>1038</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="284" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13559,23 +13550,41 @@
       <c r="B284" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C284" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D284" s="16" t="s">
+      <c r="C284" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F284" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E284" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F284" s="16" t="s">
+      <c r="G284" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K284" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L284" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="M284" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G284" s="16" t="s">
-        <v>565</v>
-      </c>
-      <c r="K284" s="16" t="s">
-        <v>477</v>
+      <c r="N284" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="O284" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="P284" s="8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="Q284" s="2" t="s">
+        <v>1038</v>
       </c>
     </row>
     <row r="285" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13585,32 +13594,23 @@
       <c r="B285" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C285" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D285" s="2" t="s">
-        <v>197</v>
+      <c r="C285" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D285" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F285" s="2" t="s">
-        <v>1031</v>
-      </c>
-      <c r="G285" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="K285" s="2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L285" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="M285" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="O285" s="2" t="s">
-        <v>1040</v>
+        <v>2</v>
+      </c>
+      <c r="F285" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="G285" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="K285" s="16" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="286" spans="1:17" ht="18" x14ac:dyDescent="0.25">
@@ -13624,27 +13624,62 @@
         <v>2</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E286" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F286" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G286" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K286" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L286" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="M286" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O286" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="287" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F287" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G286" s="2" t="s">
+      <c r="G287" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K286" s="2" t="s">
+      <c r="K287" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="L286" s="2" t="s">
+      <c r="L287" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M286" s="2" t="s">
+      <c r="M287" s="2" t="s">
         <v>1042</v>
       </c>
-      <c r="O286" s="2" t="s">
+      <c r="O287" s="2" t="s">
         <v>1043</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TS Template,TS 4.7 Jatai working 12/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Rule Processing Table.xlsx
+++ b/TS Jatai Working/Rule Processing Table.xlsx
@@ -3871,10 +3871,10 @@
   <dimension ref="A3:V291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="17" spans="1:20" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
-        <v>20</v>
+        <v>1109</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Samita & PP TS 2.5 plus Jatai Rule TTD 17/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Rule Processing Table.xlsx
+++ b/TS Jatai Working/Rule Processing Table.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1122">
   <si>
     <t>Special Rules Tables for Rajadhiraaja</t>
   </si>
@@ -3408,6 +3408,9 @@
   </si>
   <si>
     <t>uvu saH</t>
+  </si>
+  <si>
+    <t>n or an</t>
   </si>
 </sst>
 </file>
@@ -3562,7 +3565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3618,6 +3621,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3901,10 +3905,10 @@
   <dimension ref="A3:V297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E279" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F285" sqref="F285"/>
+      <selection pane="bottomRight" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8832,8 +8836,8 @@
       <c r="E147" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="2" t="s">
-        <v>39</v>
+      <c r="F147" s="37" t="s">
+        <v>1121</v>
       </c>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -8865,8 +8869,8 @@
       <c r="E148" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F148" s="2" t="s">
-        <v>39</v>
+      <c r="F148" s="37" t="s">
+        <v>1121</v>
       </c>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
@@ -8907,8 +8911,8 @@
       <c r="E149" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F149" s="2" t="s">
-        <v>39</v>
+      <c r="F149" s="37" t="s">
+        <v>1121</v>
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -8940,8 +8944,8 @@
       <c r="E150" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F150" s="2" t="s">
-        <v>39</v>
+      <c r="F150" s="37" t="s">
+        <v>1121</v>
       </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>

</xml_diff>